<commit_message>
Upto PQ challenge 20 has been solved.
</commit_message>
<xml_diff>
--- a/Excel Files/PQ Challenges/PQ Challenge 13 Problem.xlsx
+++ b/Excel Files/PQ Challenges/PQ Challenge 13 Problem.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PQ Challenges\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\Excel-BI-Python\Excel Files\PQ Challenges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{51958CB8-2061-4F48-AB80-185161BDA330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4223492-436E-4CE2-B648-A0DBA4FBE5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41148" yWindow="1536" windowWidth="23304" windowHeight="12624" xr2:uid="{42A06BE4-A360-44AD-88EB-49737251321E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{42A06BE4-A360-44AD-88EB-49737251321E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -893,13 +915,42 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="1685" row="10">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{72C62670-E3E0-4379-949A-097CBFF9C084}">
+  <we:reference id="wa200003696" version="1.2.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="WA200003696" version="1.2.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties>
+    <we:property name="projectV0_1-56c6e055-265e-4713-816e-a646dbb708de" value="{&quot;kind&quot;:&quot;AFEJSONBlobNode&quot;,&quot;id&quot;:&quot;{8E0EE645-9C67-4F07-A9A6-BE434FCACEBC}&quot;}"/>
+  </we:properties>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{740F4586-128E-4FBF-BBAA-976E0D4F19BB}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -912,7 +963,7 @@
     <col min="6" max="6" width="14.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -929,7 +980,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -945,8 +996,18 @@
       <c r="F2" s="3">
         <v>99</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="O2" t="str" cm="1">
+        <f t="array" ref="O2:Q20">_xlfn.LAMBDA(_xlpm.Data, _xlfn.LET(_xlpm.Data2, A2:B20, _xlpm.fx_ForOne, _xlfn.LAMBDA(_xlpm.MainData,_xlpm.GroupName, _xlfn.LET(_xlpm.MainData2, A2:B20, _xlpm.GroupName2, "C", _xlpm.FilteredData, _xlfn._xlws.FILTER(_xlpm.MainData, _xlfn.CHOOSECOLS(_xlpm.MainData, 1) = _xlpm.GroupName), _xlpm.RunningTotal, _xlfn.SCAN(0, _xlfn.CHOOSECOLS(_xlpm.FilteredData, 2), _xlfn.LAMBDA(_xlpm.Acc,_xlpm.Curr, IF(_xlpm.Acc + _xlpm.Curr &lt; 0, 0, _xlpm.Acc + _xlpm.Curr))), _xlpm.Result, _xlfn.HSTACK(_xlpm.FilteredData, _xlpm.RunningTotal), _xlpm.Result)), _xlpm.UniqueGroup, _xlfn.UNIQUE(_xlfn.CHOOSECOLS(_xlpm.Data, 1)), _xlpm.Result, _xlfn.DROP(_xlfn.REDUCE("", _xlpm.UniqueGroup, _xlfn.LAMBDA(_xlpm.Acc,_xlpm.Curr, _xlfn.VSTACK(_xlpm.Acc, _xlpm.fx_ForOne(_xlpm.Data, _xlpm.Curr)))), 1), _xlpm.Result))(A2:B20)</f>
+        <v>A</v>
+      </c>
+      <c r="P2">
+        <v>99</v>
+      </c>
+      <c r="Q2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -962,8 +1023,17 @@
       <c r="F3" s="3">
         <v>161</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="O3" t="str">
+        <v>A</v>
+      </c>
+      <c r="P3">
+        <v>62</v>
+      </c>
+      <c r="Q3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -979,8 +1049,17 @@
       <c r="F4" s="3">
         <v>203</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="O4" t="str">
+        <v>A</v>
+      </c>
+      <c r="P4">
+        <v>42</v>
+      </c>
+      <c r="Q4">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -996,8 +1075,17 @@
       <c r="F5" s="3">
         <v>61</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="O5" t="str">
+        <v>B</v>
+      </c>
+      <c r="P5">
+        <v>61</v>
+      </c>
+      <c r="Q5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1013,8 +1101,17 @@
       <c r="F6" s="3">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="O6" t="str">
+        <v>C</v>
+      </c>
+      <c r="P6">
+        <v>48</v>
+      </c>
+      <c r="Q6">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1030,8 +1127,17 @@
       <c r="F7" s="3">
         <v>69</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="O7" t="str">
+        <v>C</v>
+      </c>
+      <c r="P7">
+        <v>21</v>
+      </c>
+      <c r="Q7">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -1047,8 +1153,17 @@
       <c r="F8" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="O8" t="str">
+        <v>C</v>
+      </c>
+      <c r="P8">
+        <v>-81</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -1064,8 +1179,17 @@
       <c r="F9" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="O9" t="str">
+        <v>C</v>
+      </c>
+      <c r="P9">
+        <v>30</v>
+      </c>
+      <c r="Q9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -1081,8 +1205,17 @@
       <c r="F10" s="3">
         <v>52</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="O10" t="str">
+        <v>C</v>
+      </c>
+      <c r="P10">
+        <v>22</v>
+      </c>
+      <c r="Q10">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
@@ -1098,8 +1231,17 @@
       <c r="F11" s="3">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="O11" t="str">
+        <v>C</v>
+      </c>
+      <c r="P11">
+        <v>-31</v>
+      </c>
+      <c r="Q11">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -1115,8 +1257,17 @@
       <c r="F12" s="3">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="O12" t="str">
+        <v>D</v>
+      </c>
+      <c r="P12">
+        <v>16</v>
+      </c>
+      <c r="Q12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
@@ -1132,8 +1283,17 @@
       <c r="F13" s="3">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="O13" t="str">
+        <v>D</v>
+      </c>
+      <c r="P13">
+        <v>16</v>
+      </c>
+      <c r="Q13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
@@ -1149,8 +1309,17 @@
       <c r="F14" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="O14" t="str">
+        <v>D</v>
+      </c>
+      <c r="P14">
+        <v>-95</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -1166,8 +1335,17 @@
       <c r="F15" s="3">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="O15" t="str">
+        <v>D</v>
+      </c>
+      <c r="P15">
+        <v>16</v>
+      </c>
+      <c r="Q15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>6</v>
       </c>
@@ -1183,8 +1361,17 @@
       <c r="F16" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="O16" t="str">
+        <v>D</v>
+      </c>
+      <c r="P16">
+        <v>-76</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
@@ -1200,8 +1387,17 @@
       <c r="F17" s="3">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="O17" t="str">
+        <v>D</v>
+      </c>
+      <c r="P17">
+        <v>26</v>
+      </c>
+      <c r="Q17">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>6</v>
       </c>
@@ -1217,8 +1413,17 @@
       <c r="F18" s="3">
         <v>92</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="O18" t="str">
+        <v>D</v>
+      </c>
+      <c r="P18">
+        <v>66</v>
+      </c>
+      <c r="Q18">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>6</v>
       </c>
@@ -1234,8 +1439,17 @@
       <c r="F19" s="3">
         <v>82</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="O19" t="str">
+        <v>D</v>
+      </c>
+      <c r="P19">
+        <v>-10</v>
+      </c>
+      <c r="Q19">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>6</v>
       </c>
@@ -1249,6 +1463,15 @@
         <v>67</v>
       </c>
       <c r="F20" s="3">
+        <v>149</v>
+      </c>
+      <c r="O20" t="str">
+        <v>D</v>
+      </c>
+      <c r="P20">
+        <v>67</v>
+      </c>
+      <c r="Q20">
         <v>149</v>
       </c>
     </row>
@@ -1257,4 +1480,16 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHMAdABhAHQAZQBtAGUAbgB0AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAcgBvAHcAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBjAG8AbAB1AG0AbgBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFMAZQBwAGEAcgBhAHQAbwByACIAOgAiACwAIgAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAE0ARABZACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAbABvAGMAYQBsAGUATgBhAG0AZQAiADoAIgBlAG4ALQB1AHMAIgAsACIAdABoAG8AdQBzAGEAbgBkAHMAUABvAHMAaQB0AGkAbwBuAHMAIgA6AFsAMwBdAH0AfQA=</AFEJSONBlob>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E0EE645-9C67-4F07-A9A6-BE434FCACEBC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>